<commit_message>
Creating Company Stock History Worksheets
</commit_message>
<xml_diff>
--- a/StocksReport/Stocks_Report_Template.xlsx
+++ b/StocksReport/Stocks_Report_Template.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moliveira\Documents\GitHub\GrapeCityFinanceReportNet5\StocksReport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388304AF-4700-4E37-88FA-F540A3012826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F18F99-377D-402A-8EC1-FF03E51A2952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2505" yWindow="2910" windowWidth="15495" windowHeight="7545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stocks Portfolios" sheetId="1" r:id="rId1"/>
+    <sheet name="{{ds.Symbol}}" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Symbol</t>
   </si>
@@ -91,16 +92,44 @@
   </si>
   <si>
     <t xml:space="preserve">            Stocks Report</t>
+  </si>
+  <si>
+    <t>Total Cost:</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Month-Year</t>
+  </si>
+  <si>
+    <t>Price Growth (%)</t>
+  </si>
+  <si>
+    <t>Price History - {{ds.Symbol}}</t>
+  </si>
+  <si>
+    <t>{{ds.PriceHistory.PriceDate}}</t>
+  </si>
+  <si>
+    <t>{{ds.PriceHistory.PriceMonth}}</t>
+  </si>
+  <si>
+    <t>{{ds.PriceHistory.Price}}</t>
+  </si>
+  <si>
+    <t>{{ds.PriceHistory.PriceGrowth}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="171" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +207,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Lucida Sans"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -217,7 +253,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -245,12 +281,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -271,10 +317,25 @@
     <xf numFmtId="44" fontId="7" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="171" fontId="7" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -719,6 +780,473 @@
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                   <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4D9570D-50F7-4F48-800F-0D39E1A173EC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr>
+              <a:cxnSpLocks/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8685290" y="5248423"/>
+              <a:ext cx="0" cy="802446"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:grpFill/>
+            <a:ln w="63500">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+      </xdr:grpSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>811696</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>682479</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="Group 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5A7EBD0-EEB2-40B0-8C0F-CCCEF1D75181}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="76200" y="66675"/>
+          <a:ext cx="735496" cy="615804"/>
+          <a:chOff x="76200" y="66675"/>
+          <a:chExt cx="735496" cy="615804"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="3" name="Graphic 2" descr="Upward trend">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8678B22F-F7E9-40F1-BD4E-73BA65F9EFA7}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill rotWithShape="1">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect l="22504" t="30454" r="7783" b="22928"/>
+          <a:stretch/>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="112303" y="66675"/>
+            <a:ext cx="650267" cy="433715"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="4" name="Group 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BA54569-B8C4-49A2-BCB9-7B8737CDE1A3}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="76200" y="66676"/>
+            <a:ext cx="735496" cy="615803"/>
+            <a:chOff x="3825366" y="972636"/>
+            <a:chExt cx="2290916" cy="1923129"/>
+          </a:xfrm>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </xdr:grpSpPr>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="12" name="Straight Connector 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{823ED796-68D1-4859-96ED-4DC4BD447336}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr>
+              <a:cxnSpLocks/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3850498" y="972636"/>
+              <a:ext cx="16813" cy="1923129"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:grpFill/>
+            <a:ln w="50800">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="13" name="Straight Connector 12">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50F2E794-99E8-4EB6-A993-D42E6BCD2FEB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr>
+              <a:cxnSpLocks/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm flipH="1">
+              <a:off x="3825366" y="2847075"/>
+              <a:ext cx="2290916" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:grpFill/>
+            <a:ln w="50800">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+      </xdr:grpSp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="5" name="Group 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC67358B-3673-46A1-A401-F42E63C0D125}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="205950" y="255578"/>
+            <a:ext cx="512427" cy="368877"/>
+            <a:chOff x="7858218" y="5248423"/>
+            <a:chExt cx="827072" cy="802447"/>
+          </a:xfrm>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </xdr:grpSpPr>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="6" name="Straight Connector 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8639B47A-7B02-4626-A02D-ED7BC349E267}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr>
+              <a:cxnSpLocks/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8023633" y="5485329"/>
+              <a:ext cx="0" cy="565541"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:grpFill/>
+            <a:ln w="63500">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="7" name="Straight Connector 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB460C8F-AE02-480C-A121-C21BB9682A33}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr>
+              <a:cxnSpLocks/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8354462" y="5381174"/>
+              <a:ext cx="0" cy="669696"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:grpFill/>
+            <a:ln w="63500">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="8" name="Straight Connector 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F753920E-8D06-4CBE-8683-86C67B2B494D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr>
+              <a:cxnSpLocks/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8189047" y="5540656"/>
+              <a:ext cx="0" cy="510213"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:grpFill/>
+            <a:ln w="63500">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="9" name="Straight Connector 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{236972A7-6142-489C-8A1D-D48AA2DA559C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr>
+              <a:cxnSpLocks/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7858218" y="5647082"/>
+              <a:ext cx="0" cy="403787"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:grpFill/>
+            <a:ln w="63500">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="10" name="Straight Connector 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAA263EF-7640-412F-8DA1-48220AE2A927}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr>
+              <a:cxnSpLocks/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8519876" y="5485329"/>
+              <a:ext cx="0" cy="565541"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:grpFill/>
+            <a:ln w="63500">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="11" name="Straight Connector 10">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B59AD9E-ADBD-4101-B92F-D3DA65AAF1B4}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1086,8 +1614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1176,8 +1704,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="15">
+        <f>SUM(G7:G7)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" s="2"/>
@@ -1192,4 +1729,104 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{346B9099-A1BE-4071-8AD0-4592CC3707D8}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="17" style="5" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+    </row>
+    <row r="3" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:9" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="4"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="2"/>
+      <c r="D10" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Creating a Stock Price Growth Chart
</commit_message>
<xml_diff>
--- a/StocksReport/Stocks_Report_Template.xlsx
+++ b/StocksReport/Stocks_Report_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moliveira\Documents\GitHub\GrapeCityFinanceReportNet5\StocksReport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E51289-081C-4871-B65D-58C4850D8700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859ACC3E-388B-4EC4-8F78-190FFEB87C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2505" yWindow="2910" windowWidth="13185" windowHeight="5820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stocks Portfolios" sheetId="1" r:id="rId1"/>
@@ -122,10 +122,10 @@
     <t>{{ds.PriceHistory.PriceGrowth}}</t>
   </si>
   <si>
-    <t>Compared Price Growth</t>
+    <t>{{ds.Symbol(E=H)}}</t>
   </si>
   <si>
-    <t>{{ds.Symbol(E=H)}}</t>
+    <t>Compared Price Growth (%)</t>
   </si>
 </sst>
 </file>
@@ -364,6 +364,901 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Stock Price Growth (%)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Price Growth'!$C$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>{{ds.Symbol(E=H)}}</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Price Growth'!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>{{ds.PriceHistory.PriceMonth}}</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Price Growth'!$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2D0A-43BA-8E66-534AF854AA0D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1905051983"/>
+        <c:axId val="1905056559"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1905051983"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1905056559"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="20"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1905056559"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1905051983"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1760,6 +2655,42 @@
         </xdr:cxnSp>
       </xdr:grpSp>
     </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>195262</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="Chart 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{942C16C4-6129-4DB1-98B9-74D238AA96BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2309,8 +3240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{161E4612-E4E8-42EA-95F6-FCAB01CDF46A}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2318,7 +3249,7 @@
     <col min="1" max="1" width="45.42578125" style="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.140625" style="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.85546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="17" customWidth="1"/>
     <col min="5" max="9" width="17" style="17" customWidth="1"/>
     <col min="10" max="10" width="10.28515625" style="17" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5703125" style="17" bestFit="1" customWidth="1"/>
@@ -2341,7 +3272,7 @@
     </row>
     <row r="3" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -2353,7 +3284,7 @@
         <v>22</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>

</xml_diff>